<commit_message>
add labels for packings
</commit_message>
<xml_diff>
--- a/app/data/static/samples/by_department/mascarpone/sample_schedule.xlsx
+++ b/app/data/static/samples/by_department/mascarpone/sample_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Documents/coding/repos/umalat/app/data/static/samples/by_department/mascarpone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF44262-C327-B249-8387-570C74470FE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7735BD62-72F9-E944-8D7B-441F72F5F244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12361,7 +12361,7 @@
   <dimension ref="A1:S339"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12716,7 +12716,7 @@
         <v>4000</v>
       </c>
       <c r="I10" s="30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J10" s="30" t="s">
         <v>371</v>

</xml_diff>

<commit_message>
fix 0.14 ->0.18 switch
</commit_message>
<xml_diff>
--- a/app/data/static/samples/by_department/mascarpone/sample_schedule.xlsx
+++ b/app/data/static/samples/by_department/mascarpone/sample_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marklidenberg/Documents/coding/repos/umalat/app/data/static/samples/by_department/mascarpone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7735BD62-72F9-E944-8D7B-441F72F5F244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B96755-DACB-5549-AE63-660557AE587E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="файл остатки" sheetId="1" r:id="rId1"/>
     <sheet name="планирование суточное" sheetId="2" r:id="rId2"/>
     <sheet name="План варок" sheetId="3" r:id="rId3"/>
-    <sheet name="SKU Маскарпоне" sheetId="4" state="hidden" r:id="rId4"/>
+    <sheet name="SKU Маскарпоне" sheetId="4" r:id="rId4"/>
     <sheet name="Заквасочники" sheetId="5" state="hidden" r:id="rId5"/>
     <sheet name="SKU заквасочник" sheetId="6" state="hidden" r:id="rId6"/>
     <sheet name="Расписание" sheetId="7" r:id="rId7"/>
@@ -12360,8 +12360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S339"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13036,8 +13036,8 @@
       <c r="C19" s="40" t="s">
         <v>323</v>
       </c>
-      <c r="D19" s="39" t="s">
-        <v>102</v>
+      <c r="D19" s="30" t="s">
+        <v>103</v>
       </c>
       <c r="E19" s="41">
         <v>1200</v>
@@ -18807,7 +18807,7 @@
   <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>